<commit_message>
Final column names for GCHeadspace and Key templates
</commit_message>
<xml_diff>
--- a/Synoptic/Template_GHG_Key.xlsx
+++ b/Synoptic/Template_GHG_Key.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carla López Lloreda\Dropbox\Grad school\Research\Delmarva project\Data\Synoptic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A0F87FF-0FEA-4733-B7EE-0705D183988A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFC1F1D-34F7-49C1-BBE4-55BBB72698B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F038E0C-33BA-477A-BCDB-AAA57BAAF801}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,16 +57,16 @@
     <t>GC_Notes</t>
   </si>
   <si>
-    <t>Water_Temp_DegC</t>
-  </si>
-  <si>
-    <t>Ambient_air</t>
-  </si>
-  <si>
     <t>Flag</t>
   </si>
   <si>
     <t>Flag_notes</t>
+  </si>
+  <si>
+    <t>Air_Location</t>
+  </si>
+  <si>
+    <t>Water_Temp_C</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,6 +439,7 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.109375" customWidth="1"/>
     <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -464,16 +465,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>